<commit_message>
Review Pivot Report of pabi_utils
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_advance_status.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_advance_status.xlsx
@@ -22,7 +22,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">รายงานลูกหนี้เงินยืมทดรองจ่าย</t>
+  </si>
   <si>
     <t xml:space="preserve">สิ้นสุดวันที่</t>
   </si>
@@ -132,9 +135,6 @@
     <t xml:space="preserve">เงินยืมคงค้าง</t>
   </si>
   <si>
-    <t xml:space="preserve">รายงานลูกหนี้เงินยืมทดรองจ่าย</t>
-  </si>
-  <si>
     <t xml:space="preserve">1 - 15 วัน</t>
   </si>
   <si>
@@ -147,7 +147,7 @@
     <t xml:space="preserve">รวมทั้งหมด</t>
   </si>
   <si>
-    <t xml:space="preserve">รายละเอียดรายงานลูกหนี้เงินยืมทดรองจ่าย</t>
+    <t xml:space="preserve">รายงานรายละเอียดลูกหนี้เงินยืมทดรองจ่าย</t>
   </si>
   <si>
     <t xml:space="preserve">พนักงาน</t>
@@ -186,6 +186,12 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="14"/>
+      <name val="FreeSans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="FreeSans"/>
       <family val="2"/>
@@ -195,13 +201,6 @@
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <name val="FreeSans"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -293,7 +292,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -306,15 +305,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -322,31 +329,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -437,8 +428,8 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -458,61 +449,64 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5"/>
       <c r="E2" s="1"/>
-      <c r="J2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="6"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="K3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="L3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="M3" s="7" t="s">
         <v>16</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -534,56 +528,53 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="10" width="25.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="11" width="25.55"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <f aca="false">'Advance Status Report'!B1</f>
-        <v>0</v>
-      </c>
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -612,58 +603,55 @@
   <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="10" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="11" width="27.31"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="2" t="n">
-        <f aca="false">'Advance Status Report'!B1</f>
-        <v>0</v>
-      </c>
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>